<commit_message>
Adding filtering of accepted orders to reject negative profit ones. Increases profit by 50%. Updating evaluation files.
</commit_message>
<xml_diff>
--- a/MAC Worskpace - Multi-Agent/Coursework_SET10111/base_log_data.xlsx
+++ b/MAC Worskpace - Multi-Agent/Coursework_SET10111/base_log_data.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,40 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zsoltvarga/Napier/2019-2020/Trimester_1_(y4)/Multi-Agent Systems/Multi-Agent_Systems-Module/MAC Worskpace - Multi-Agent/Coursework_SET10111/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{91051B63-BFDB-074B-80D7-C9C45712AD3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9312A951-D536-F046-AC53-E764767654F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="1660" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="1420" yWindow="840" windowWidth="31820" windowHeight="19440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="base_log_data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">base_log_data!$C$2:$C$31</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">base_log_data!$C$2:$C$31</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">base_log_data!$C$35:$C$63</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">base_log_data!$C$2:$C$31</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">base_log_data!$C$34</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">base_log_data!$C$35:$C$63</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">base_log_data!$C$2:$C$31</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">base_log_data!$C$34</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">base_log_data!$C$35:$C$63</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">base_log_data!$C$2:$C$31</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">base_log_data!$C$34</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
   <si>
     <t>customers</t>
   </si>
@@ -31,13 +52,25 @@
     <t>profit</t>
   </si>
   <si>
-    <t>average profit</t>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>SEM</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>Most times the manufacturer profited £406,598.20  +- 17%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -515,8 +548,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -573,6 +607,1512 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.0</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>Performance with base configuration</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>Performance with base configuration</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" uniqueId="{A9D12DF0-5455-D947-8185-C17391B6E32E}" formatIdx="0">
+          <cx:tx>
+            <cx:txData>
+              <cx:f/>
+              <cx:v>Profit</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:spPr>
+            <a:noFill/>
+          </cx:spPr>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="1" meanMarker="1" nonoutliers="1" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0" hidden="1">
+        <cx:catScaling gapWidth="1"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:title>
+          <cx:tx>
+            <cx:txData>
+              <cx:v>Profit</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:txPr>
+            <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr sz="1200"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+                </a:rPr>
+                <a:t>Profit</a:t>
+              </a:r>
+            </a:p>
+          </cx:txPr>
+        </cx:title>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+        <cx:numFmt formatCode="£#,##0" sourceLinked="0"/>
+        <cx:txPr>
+          <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr" rtl="0">
+              <a:defRPr sz="1000"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-GB" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:endParaRPr>
+          </a:p>
+        </cx:txPr>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx2.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.10</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>Performance with base configuration</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>Performance with base configuration</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" uniqueId="{C846A100-F5CA-EB4B-8ED4-22F1CE72517B}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.9</cx:f>
+              <cx:v>profit</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:spPr>
+            <a:noFill/>
+          </cx:spPr>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0" hidden="1">
+        <cx:catScaling gapWidth="1"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:title>
+          <cx:tx>
+            <cx:txData>
+              <cx:v>Profit</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:txPr>
+            <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr sz="1200"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+                </a:rPr>
+                <a:t>Profit</a:t>
+              </a:r>
+            </a:p>
+          </cx:txPr>
+        </cx:title>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+        <cx:numFmt formatCode="£#,##0" sourceLinked="0"/>
+        <cx:txPr>
+          <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr" rtl="0">
+              <a:defRPr sz="1000"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-GB" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:endParaRPr>
+          </a:p>
+        </cx:txPr>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>91440</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>121921</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>20320</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="2" name="Chart 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41C72391-73E0-BD4B-855B-582EC3D719E9}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3393440" y="1747521"/>
+              <a:ext cx="4124960" cy="3149599"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100"/>
+                <a:t>This chart isn’t available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>256325</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>136989</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>825285</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>35388</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="3" name="Chart 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1DF9BF64-5A7F-A748-B21D-86BD7C823695}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3558325" y="8264989"/>
+              <a:ext cx="4124960" cy="3149599"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100"/>
+                <a:t>This chart isn’t available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -871,20 +2411,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="107" zoomScaleNormal="122" workbookViewId="0">
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="5" width="10.33203125" customWidth="1"/>
     <col min="6" max="6" width="13.83203125" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="1"/>
+    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -894,8 +2437,17 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>3</v>
       </c>
@@ -905,14 +2457,20 @@
       <c r="C2">
         <v>474230</v>
       </c>
-      <c r="E2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F2">
+        <f>AVERAGE(C2:C31)</f>
+        <v>406598.2</v>
+      </c>
+      <c r="G2">
+        <f>STDEV(C2:C31)</f>
+        <v>69118.088660614347</v>
+      </c>
+      <c r="H2">
+        <f>G2/(SQRT(30))</f>
+        <v>12619.178763686838</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>3</v>
       </c>
@@ -922,15 +2480,8 @@
       <c r="C3">
         <v>490527</v>
       </c>
-      <c r="E3">
-        <v>3</v>
-      </c>
-      <c r="F3">
-        <f>AVERAGE(C2:C31)</f>
-        <v>406598.2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -941,7 +2492,7 @@
         <v>386883</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -951,8 +2502,15 @@
       <c r="C5">
         <v>444988</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H5">
+        <f>G2/F2*100</f>
+        <v>16.999113291847909</v>
+      </c>
+      <c r="I5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3</v>
       </c>
@@ -962,8 +2520,11 @@
       <c r="C6">
         <v>374347</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3</v>
       </c>
@@ -974,7 +2535,7 @@
         <v>479784</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>3</v>
       </c>
@@ -985,7 +2546,7 @@
         <v>406749</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>3</v>
       </c>
@@ -996,7 +2557,7 @@
         <v>389212</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>3</v>
       </c>
@@ -1007,7 +2568,7 @@
         <v>607443</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>3</v>
       </c>
@@ -1018,7 +2579,7 @@
         <v>295730</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>3</v>
       </c>
@@ -1029,7 +2590,7 @@
         <v>383235</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>3</v>
       </c>
@@ -1040,7 +2601,7 @@
         <v>360921</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>3</v>
       </c>
@@ -1051,7 +2612,7 @@
         <v>277622</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>3</v>
       </c>
@@ -1062,7 +2623,7 @@
         <v>378899</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>3</v>
       </c>
@@ -1236,10 +2797,380 @@
       </c>
       <c r="C31">
         <v>381251</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s">
+        <v>2</v>
+      </c>
+      <c r="F34" t="s">
+        <v>5</v>
+      </c>
+      <c r="G34" t="s">
+        <v>3</v>
+      </c>
+      <c r="H34" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>3</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>650235</v>
+      </c>
+      <c r="F35">
+        <f>AVERAGE(C35:C64)</f>
+        <v>628937.69999999995</v>
+      </c>
+      <c r="G35">
+        <f>STDEV(C35:C64)</f>
+        <v>67504.008848083206</v>
+      </c>
+      <c r="H35">
+        <f>G35/(SQRT(30))</f>
+        <v>12324.489456041165</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>3</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>633308</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>3</v>
+      </c>
+      <c r="B37">
+        <v>2</v>
+      </c>
+      <c r="C37">
+        <v>670348</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>3</v>
+      </c>
+      <c r="B38">
+        <v>3</v>
+      </c>
+      <c r="C38">
+        <v>603401</v>
+      </c>
+      <c r="H38">
+        <f>G35/F35*100</f>
+        <v>10.733019955407858</v>
+      </c>
+      <c r="I38" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>3</v>
+      </c>
+      <c r="B39">
+        <v>4</v>
+      </c>
+      <c r="C39">
+        <v>666844</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>3</v>
+      </c>
+      <c r="B40">
+        <v>5</v>
+      </c>
+      <c r="C40">
+        <v>689566</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>3</v>
+      </c>
+      <c r="B41">
+        <v>6</v>
+      </c>
+      <c r="C41">
+        <v>635974</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>3</v>
+      </c>
+      <c r="B42">
+        <v>7</v>
+      </c>
+      <c r="C42">
+        <v>683250</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>3</v>
+      </c>
+      <c r="B43">
+        <v>8</v>
+      </c>
+      <c r="C43">
+        <v>555760</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>3</v>
+      </c>
+      <c r="B44">
+        <v>9</v>
+      </c>
+      <c r="C44">
+        <v>612781</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>3</v>
+      </c>
+      <c r="B45">
+        <v>10</v>
+      </c>
+      <c r="C45">
+        <v>528768</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>3</v>
+      </c>
+      <c r="B46">
+        <v>11</v>
+      </c>
+      <c r="C46">
+        <v>670275</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>3</v>
+      </c>
+      <c r="B47">
+        <v>12</v>
+      </c>
+      <c r="C47">
+        <v>711791</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>3</v>
+      </c>
+      <c r="B48">
+        <v>13</v>
+      </c>
+      <c r="C48">
+        <v>742790</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>3</v>
+      </c>
+      <c r="B49">
+        <v>14</v>
+      </c>
+      <c r="C49">
+        <v>682269</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>3</v>
+      </c>
+      <c r="B50">
+        <v>15</v>
+      </c>
+      <c r="C50">
+        <v>689283</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>3</v>
+      </c>
+      <c r="B51">
+        <v>16</v>
+      </c>
+      <c r="C51">
+        <v>532485</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>3</v>
+      </c>
+      <c r="B52">
+        <v>17</v>
+      </c>
+      <c r="C52">
+        <v>526666</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>3</v>
+      </c>
+      <c r="B53">
+        <v>18</v>
+      </c>
+      <c r="C53">
+        <v>554139</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>3</v>
+      </c>
+      <c r="B54">
+        <v>19</v>
+      </c>
+      <c r="C54">
+        <v>713210</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>3</v>
+      </c>
+      <c r="B55">
+        <v>20</v>
+      </c>
+      <c r="C55">
+        <v>710909</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>3</v>
+      </c>
+      <c r="B56">
+        <v>21</v>
+      </c>
+      <c r="C56">
+        <v>618929</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>3</v>
+      </c>
+      <c r="B57">
+        <v>22</v>
+      </c>
+      <c r="C57">
+        <v>596934</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>3</v>
+      </c>
+      <c r="B58">
+        <v>23</v>
+      </c>
+      <c r="C58">
+        <v>555588</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>3</v>
+      </c>
+      <c r="B59">
+        <v>24</v>
+      </c>
+      <c r="C59">
+        <v>570584</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>3</v>
+      </c>
+      <c r="B60">
+        <v>25</v>
+      </c>
+      <c r="C60">
+        <v>490377</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>3</v>
+      </c>
+      <c r="B61">
+        <v>26</v>
+      </c>
+      <c r="C61">
+        <v>647062</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>3</v>
+      </c>
+      <c r="B62">
+        <v>27</v>
+      </c>
+      <c r="C62">
+        <v>663227</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>3</v>
+      </c>
+      <c r="B63">
+        <v>28</v>
+      </c>
+      <c r="C63">
+        <v>568536</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>3</v>
+      </c>
+      <c r="B64">
+        <v>29</v>
+      </c>
+      <c r="C64">
+        <v>692842</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate function="average"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>